<commit_message>
21 Sept 2016 : 3:10 pm :: Second code change to incorporate the change in the datafile path in Constant.java as a result of the Project location change.
</commit_message>
<xml_diff>
--- a/HybridFramework/src/main/java/dataEngine/DataEngine.xlsx
+++ b/HybridFramework/src/main/java/dataEngine/DataEngine.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="86">
   <si>
     <t>Description</t>
   </si>
@@ -283,6 +283,9 @@
   </si>
   <si>
     <t>No</t>
+  </si>
+  <si>
+    <t>FAIL</t>
   </si>
 </sst>
 </file>
@@ -749,7 +752,7 @@
         <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -1259,7 +1262,7 @@
       </c>
       <c r="G19" s="5"/>
       <c r="H19" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
22-Sep-2016 : 3rd code change To incorporate the screenshot functionality
</commit_message>
<xml_diff>
--- a/HybridFramework/src/main/java/dataEngine/DataEngine.xlsx
+++ b/HybridFramework/src/main/java/dataEngine/DataEngine.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23970" windowHeight="9810"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23970" windowHeight="9810" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="85">
   <si>
     <t>Description</t>
   </si>
@@ -280,9 +280,6 @@
   </si>
   <si>
     <t>PASS</t>
-  </si>
-  <si>
-    <t>No</t>
   </si>
   <si>
     <t>FAIL</t>
@@ -701,8 +698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -735,7 +732,7 @@
         <v>32</v>
       </c>
       <c r="C2" s="1" t="s">
-        <v>84</v>
+        <v>18</v>
       </c>
       <c r="D2" t="s">
         <v>83</v>
@@ -752,7 +749,7 @@
         <v>18</v>
       </c>
       <c r="D3" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="30" x14ac:dyDescent="0.25">
@@ -763,7 +760,7 @@
         <v>40</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>84</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
         <v>83</v>
@@ -779,8 +776,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2:H34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1192,7 +1189,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>38</v>
       </c>
@@ -1219,7 +1216,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>38</v>
       </c>
@@ -1243,7 +1240,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>38</v>
       </c>
@@ -1262,10 +1259,10 @@
       </c>
       <c r="G19" s="5"/>
       <c r="H19" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>39</v>
       </c>
@@ -1290,7 +1287,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>39</v>
       </c>
@@ -1315,7 +1312,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>39</v>
       </c>
@@ -1339,7 +1336,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>39</v>
       </c>
@@ -1366,7 +1363,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>39</v>
       </c>
@@ -1390,7 +1387,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>39</v>
       </c>
@@ -1414,7 +1411,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>39</v>
       </c>
@@ -1441,7 +1438,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>39</v>
       </c>
@@ -1465,7 +1462,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>39</v>
       </c>

</xml_diff>

<commit_message>
22 Sept 2016 : 9:12 pm - Fourth code change To make the screenshot functionality more robust and user friendly.
</commit_message>
<xml_diff>
--- a/HybridFramework/src/main/java/dataEngine/DataEngine.xlsx
+++ b/HybridFramework/src/main/java/dataEngine/DataEngine.xlsx
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="267" uniqueCount="85">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="380" uniqueCount="85">
   <si>
     <t>Description</t>
   </si>
@@ -763,7 +763,7 @@
         <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
   </sheetData>
@@ -1087,7 +1087,7 @@
         <v>http://mail.yahoo.com/</v>
       </c>
       <c r="H12" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
@@ -1213,7 +1213,7 @@
         <v>finland1234</v>
       </c>
       <c r="H17" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
@@ -1309,7 +1309,7 @@
         <v>http://mail.yahoo.com/</v>
       </c>
       <c r="H21" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>